<commit_message>
Export Evaluationsmatrix und import XML auszug
</commit_message>
<xml_diff>
--- a/Files/Tabellen/Export-Evaluationsmatrix.xlsx
+++ b/Files/Tabellen/Export-Evaluationsmatrix.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Kriterium</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t>PDF gewichtet</t>
+  </si>
+  <si>
+    <t>Darstellungsmöglichkeiten</t>
+  </si>
+  <si>
+    <t>Einfache Handhabung</t>
+  </si>
+  <si>
+    <t>Kosten</t>
   </si>
 </sst>
 </file>
@@ -219,6 +228,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -227,8 +238,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -501,7 +510,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -512,7 +521,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,7 +552,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="1">
@@ -565,49 +574,73 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="A3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1">
+        <v>10</v>
+      </c>
       <c r="E3" s="2">
         <f t="shared" ref="E3:E6" si="0">B3*C3</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F3" s="2">
         <f t="shared" ref="F3:F6" si="1">D3*B3</f>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="A4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1">
+        <v>10</v>
+      </c>
       <c r="E4" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1">
+        <v>8</v>
+      </c>
       <c r="E5" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="3">
@@ -629,33 +662,33 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="10"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="5">
         <f>SUM(C2:C6)</f>
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="D7" s="5">
         <f>SUM(D2:D6)</f>
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="11"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="8">
         <f>SUM(E2:E6)</f>
-        <v>86</v>
+        <v>125</v>
       </c>
       <c r="D8" s="5">
         <f>SUM(F2:F6)</f>
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -664,21 +697,21 @@
       <c r="B10" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="15"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="15"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>